<commit_message>
Date validity check implemented and verified. More test cases developed.
</commit_message>
<xml_diff>
--- a/Date_calculator_console_app/date_test_data_02.xlsx
+++ b/Date_calculator_console_app/date_test_data_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git_repositories\Date_calculator_console_app\Date_calculator_console_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01B9D89-1608-4600-885D-A9BBCB7B7C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8DE069-6703-4468-9336-1B7067B913EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="1950" windowWidth="16095" windowHeight="13095" xr2:uid="{227263D0-AED4-45ED-8ED9-036391BA46B7}"/>
+    <workbookView xWindow="36135" yWindow="1005" windowWidth="17805" windowHeight="14025" xr2:uid="{227263D0-AED4-45ED-8ED9-036391BA46B7}"/>
   </bookViews>
   <sheets>
     <sheet name="date_test_data_01" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>99/99/9999</t>
+  </si>
+  <si>
+    <t>8/3/1492</t>
+  </si>
+  <si>
+    <t>10/31/1517</t>
+  </si>
+  <si>
+    <t>4/8/1492</t>
+  </si>
+  <si>
+    <t>3/31/1685</t>
+  </si>
+  <si>
+    <t>7/4/1776</t>
+  </si>
+  <si>
+    <t>12/3/1805</t>
+  </si>
+  <si>
+    <t>4/6/1830</t>
+  </si>
+  <si>
+    <t>1/1/537</t>
+  </si>
+  <si>
+    <t>4/6/1893</t>
+  </si>
+  <si>
+    <t>08/13/-1</t>
+  </si>
+  <si>
+    <t>0/22/1984</t>
+  </si>
+  <si>
+    <t>13/19/1956</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +98,17 @@
     <font>
       <sz val="11"/>
       <color rgb="FF040C28"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -86,11 +133,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,9 +456,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DABDEE-2000-4FEC-878E-9C98AAD9B175}">
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -425,27 +476,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
-        <f>MONTH(G1)</f>
+        <f t="shared" ref="A1:A35" si="0">MONTH(G1)</f>
         <v>1</v>
       </c>
       <c r="B1" s="2">
-        <f>DAY(G1)</f>
+        <f t="shared" ref="B1:B35" si="1">DAY(G1)</f>
         <v>5</v>
       </c>
       <c r="C1" s="2">
-        <f>YEAR(G1)</f>
+        <f t="shared" ref="C1:C35" si="2">YEAR(G1)</f>
         <v>1960</v>
       </c>
       <c r="D1" s="2">
-        <f>MONTH(H1)</f>
+        <f t="shared" ref="D1:D35" si="3">MONTH(H1)</f>
         <v>12</v>
       </c>
       <c r="E1" s="2">
-        <f>DAY(H1)</f>
+        <f t="shared" ref="E1:E35" si="4">DAY(H1)</f>
         <v>15</v>
       </c>
       <c r="F1" s="2">
-        <f>YEAR(H1)</f>
+        <f t="shared" ref="F1:F35" si="5">YEAR(H1)</f>
         <v>2021</v>
       </c>
       <c r="G1" s="1">
@@ -455,7 +506,7 @@
         <v>44545</v>
       </c>
       <c r="I1" s="2">
-        <f>_xlfn.DAYS(H1,G1)</f>
+        <f t="shared" ref="I1:I26" si="6">_xlfn.DAYS(H1,G1)</f>
         <v>22625</v>
       </c>
       <c r="J1" s="3">
@@ -473,27 +524,27 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <f>MONTH(G2)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <f>DAY(G2)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C2" s="2">
-        <f>YEAR(G2)</f>
+        <f t="shared" si="2"/>
         <v>1950</v>
       </c>
       <c r="D2" s="2">
-        <f>MONTH(H2)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <f>DAY(H2)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="F2" s="2">
-        <f>YEAR(H2)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G2" s="1">
@@ -503,7 +554,7 @@
         <v>36774</v>
       </c>
       <c r="I2" s="2">
-        <f>_xlfn.DAYS(H2,G2)</f>
+        <f t="shared" si="6"/>
         <v>18429</v>
       </c>
       <c r="J2" s="3">
@@ -520,27 +571,27 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <f>MONTH(G3)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <f>DAY(G3)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C3" s="2">
-        <f>YEAR(G3)</f>
+        <f t="shared" si="2"/>
         <v>1940</v>
       </c>
       <c r="D3" s="2">
-        <f>MONTH(H3)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E3" s="2">
-        <f>DAY(H3)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="F3" s="2">
-        <f>YEAR(H3)</f>
+        <f t="shared" si="5"/>
         <v>2010</v>
       </c>
       <c r="G3" s="1">
@@ -550,7 +601,7 @@
         <v>40265</v>
       </c>
       <c r="I3" s="2">
-        <f>_xlfn.DAYS(H3,G3)</f>
+        <f t="shared" si="6"/>
         <v>25299</v>
       </c>
       <c r="J3" s="3">
@@ -567,27 +618,27 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <f>MONTH(G4)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <f>DAY(G4)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C4" s="2">
-        <f>YEAR(G4)</f>
+        <f t="shared" si="2"/>
         <v>1940</v>
       </c>
       <c r="D4" s="2">
-        <f>MONTH(H4)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="E4" s="2">
-        <f>DAY(H4)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="F4" s="2">
-        <f>YEAR(H4)</f>
+        <f t="shared" si="5"/>
         <v>2020</v>
       </c>
       <c r="G4" s="1">
@@ -597,7 +648,7 @@
         <v>43956</v>
       </c>
       <c r="I4" s="2">
-        <f>_xlfn.DAYS(H4,G4)</f>
+        <f t="shared" si="6"/>
         <v>29012</v>
       </c>
       <c r="J4" s="3">
@@ -615,27 +666,27 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <f>MONTH(G5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <f>DAY(G5)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <f>YEAR(G5)</f>
+        <f t="shared" si="2"/>
         <v>1980</v>
       </c>
       <c r="D5" s="2">
-        <f>MONTH(H5)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E5" s="2">
-        <f>DAY(H5)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="F5" s="2">
-        <f>YEAR(H5)</f>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="G5" s="1">
@@ -645,7 +696,7 @@
         <v>44383</v>
       </c>
       <c r="I5" s="2">
-        <f>_xlfn.DAYS(H5,G5)</f>
+        <f t="shared" si="6"/>
         <v>14975</v>
       </c>
       <c r="J5" s="3">
@@ -660,27 +711,27 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <f>MONTH(G6)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <f>DAY(G6)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <f>YEAR(G6)</f>
+        <f t="shared" si="2"/>
         <v>1980</v>
       </c>
       <c r="D6" s="2">
-        <f>MONTH(H6)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E6" s="2">
-        <f>DAY(H6)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F6" s="2">
-        <f>YEAR(H6)</f>
+        <f t="shared" si="5"/>
         <v>2011</v>
       </c>
       <c r="G6" s="1">
@@ -690,11 +741,11 @@
         <v>40740</v>
       </c>
       <c r="I6" s="2">
-        <f>_xlfn.DAYS(H6,G6)</f>
+        <f t="shared" si="6"/>
         <v>11333</v>
       </c>
       <c r="J6" s="3">
-        <f>DATEDIF(0,I6,"y")</f>
+        <f t="shared" ref="J6:J21" si="7">DATEDIF(0,I6,"y")</f>
         <v>31</v>
       </c>
       <c r="K6" s="3">
@@ -707,27 +758,27 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <f>MONTH(G7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <f>DAY(G7)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <f>YEAR(G7)</f>
+        <f t="shared" si="2"/>
         <v>1987</v>
       </c>
       <c r="D7" s="2">
-        <f>MONTH(H7)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E7" s="2">
-        <f>DAY(H7)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F7" s="2">
-        <f>YEAR(H7)</f>
+        <f t="shared" si="5"/>
         <v>2023</v>
       </c>
       <c r="G7" s="1">
@@ -737,11 +788,11 @@
         <v>44993</v>
       </c>
       <c r="I7" s="2">
-        <f>_xlfn.DAYS(H7,G7)</f>
+        <f t="shared" si="6"/>
         <v>13141</v>
       </c>
       <c r="J7" s="3">
-        <f>DATEDIF(0,I7,"y")</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="K7" s="3">
@@ -754,27 +805,27 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <f>MONTH(G8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <f>DAY(G8)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C8" s="2">
-        <f>YEAR(G8)</f>
+        <f t="shared" si="2"/>
         <v>1994</v>
       </c>
       <c r="D8" s="2">
-        <f>MONTH(H8)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E8" s="2">
-        <f>DAY(H8)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="F8" s="2">
-        <f>YEAR(H8)</f>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="G8" s="1">
@@ -784,11 +835,11 @@
         <v>42443</v>
       </c>
       <c r="I8" s="2">
-        <f>_xlfn.DAYS(H8,G8)</f>
+        <f t="shared" si="6"/>
         <v>7944</v>
       </c>
       <c r="J8" s="3">
-        <f>DATEDIF(0,I8,"y")</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="K8" s="3">
@@ -800,27 +851,27 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f>MONTH(G9)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <f>DAY(G9)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C9" s="2">
-        <f>YEAR(G9)</f>
+        <f t="shared" si="2"/>
         <v>1953</v>
       </c>
       <c r="D9" s="2">
-        <f>MONTH(H9)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E9" s="2">
-        <f>DAY(H9)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="F9" s="2">
-        <f>YEAR(H9)</f>
+        <f t="shared" si="5"/>
         <v>1976</v>
       </c>
       <c r="G9" s="1">
@@ -830,15 +881,15 @@
         <v>27947</v>
       </c>
       <c r="I9" s="2">
-        <f>_xlfn.DAYS(H9,G9)</f>
+        <f t="shared" si="6"/>
         <v>8462</v>
       </c>
       <c r="J9" s="3">
-        <f>DATEDIF(0,I9,"y")</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="K9" s="3">
-        <f>DATEDIF(0,I9,"ym")</f>
+        <f t="shared" ref="K9:K21" si="8">DATEDIF(0,I9,"ym")</f>
         <v>2</v>
       </c>
       <c r="L9" s="3">
@@ -847,27 +898,27 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f>MONTH(G10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" s="2">
-        <f>DAY(G10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C10" s="2">
-        <f>YEAR(G10)</f>
+        <f t="shared" si="2"/>
         <v>1943</v>
       </c>
       <c r="D10" s="2">
-        <f>MONTH(H10)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E10" s="2">
-        <f>DAY(H10)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F10" s="2">
-        <f>YEAR(H10)</f>
+        <f t="shared" si="5"/>
         <v>1943</v>
       </c>
       <c r="G10" s="1">
@@ -877,15 +928,15 @@
         <v>15768</v>
       </c>
       <c r="I10" s="2">
-        <f>_xlfn.DAYS(H10,G10)</f>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="J10" s="3">
-        <f>DATEDIF(0,I10,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K10" s="3">
-        <f>DATEDIF(0,I10,"ym")</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="L10" s="3">
@@ -894,27 +945,27 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <f>MONTH(G11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B11" s="2">
-        <f>DAY(G11)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C11" s="2">
-        <f>YEAR(G11)</f>
+        <f t="shared" si="2"/>
         <v>1943</v>
       </c>
       <c r="D11" s="2">
-        <f>MONTH(H11)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E11" s="2">
-        <f>DAY(H11)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F11" s="2">
-        <f>YEAR(H11)</f>
+        <f t="shared" si="5"/>
         <v>1943</v>
       </c>
       <c r="G11" s="1">
@@ -924,15 +975,15 @@
         <v>15873</v>
       </c>
       <c r="I11" s="2">
-        <f>_xlfn.DAYS(H11,G11)</f>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="J11" s="3">
-        <f>DATEDIF(0,I11,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K11" s="3">
-        <f>DATEDIF(0,I11,"ym")</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="L11" s="3">
@@ -941,27 +992,27 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f>MONTH(G12)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B12" s="2">
-        <f>DAY(G12)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C12" s="2">
-        <f>YEAR(G12)</f>
+        <f t="shared" si="2"/>
         <v>1943</v>
       </c>
       <c r="D12" s="2">
-        <f>MONTH(H12)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E12" s="2">
-        <f>DAY(H12)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="F12" s="2">
-        <f>YEAR(H12)</f>
+        <f t="shared" si="5"/>
         <v>1943</v>
       </c>
       <c r="G12" s="1">
@@ -971,15 +1022,15 @@
         <v>15897</v>
       </c>
       <c r="I12" s="2">
-        <f>_xlfn.DAYS(H12,G12)</f>
+        <f t="shared" si="6"/>
         <v>129</v>
       </c>
       <c r="J12" s="3">
-        <f>DATEDIF(0,I12,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K12" s="3">
-        <f>DATEDIF(0,I12,"ym")</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="L12" s="3">
@@ -988,27 +1039,27 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f>MONTH(G13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B13" s="2">
-        <f>DAY(G13)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C13" s="2">
-        <f>YEAR(G13)</f>
+        <f t="shared" si="2"/>
         <v>1967</v>
       </c>
       <c r="D13" s="2">
-        <f>MONTH(H13)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="E13" s="2">
-        <f>DAY(H13)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="F13" s="2">
-        <f>YEAR(H13)</f>
+        <f t="shared" si="5"/>
         <v>1967</v>
       </c>
       <c r="G13" s="1">
@@ -1018,15 +1069,15 @@
         <v>24760</v>
       </c>
       <c r="I13" s="2">
-        <f>_xlfn.DAYS(H13,G13)</f>
+        <f t="shared" si="6"/>
         <v>237</v>
       </c>
       <c r="J13" s="3">
-        <f>DATEDIF(0,I13,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K13" s="3">
-        <f>DATEDIF(0,I13,"ym")</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="L13" s="3">
@@ -1035,27 +1086,27 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f>MONTH(G14)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <f>DAY(G14)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C14" s="2">
-        <f>YEAR(G14)</f>
+        <f t="shared" si="2"/>
         <v>2020</v>
       </c>
       <c r="D14" s="2">
-        <f>MONTH(H14)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E14" s="2">
-        <f>DAY(H14)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="F14" s="2">
-        <f>YEAR(H14)</f>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="G14" s="1">
@@ -1065,15 +1116,15 @@
         <v>44233</v>
       </c>
       <c r="I14" s="2">
-        <f>_xlfn.DAYS(H14,G14)</f>
+        <f t="shared" si="6"/>
         <v>52</v>
       </c>
       <c r="J14" s="3">
-        <f>DATEDIF(0,I14,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K14" s="3">
-        <f>DATEDIF(0,I14,"ym")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L14" s="3">
@@ -1083,27 +1134,27 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <f>MONTH(G15)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="2">
-        <f>DAY(G15)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C15" s="2">
-        <f>YEAR(G15)</f>
+        <f t="shared" si="2"/>
         <v>2020</v>
       </c>
       <c r="D15" s="2">
-        <f>MONTH(H15)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <f>DAY(H15)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="F15" s="2">
-        <f>YEAR(H15)</f>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="G15" s="1">
@@ -1113,15 +1164,15 @@
         <v>44201</v>
       </c>
       <c r="I15" s="2">
-        <f>_xlfn.DAYS(H15,G15)</f>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
       <c r="J15" s="3">
-        <f>DATEDIF(0,I15,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <f>DATEDIF(0,I15,"ym")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L15" s="3">
@@ -1130,27 +1181,27 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <f>MONTH(G16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B16" s="2">
-        <f>DAY(G16)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C16" s="2">
-        <f>YEAR(G16)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D16" s="2">
-        <f>MONTH(H16)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E16" s="2">
-        <f>DAY(H16)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F16" s="2">
-        <f>YEAR(H16)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G16" s="1">
@@ -1160,15 +1211,15 @@
         <v>36710</v>
       </c>
       <c r="I16" s="2">
-        <f>_xlfn.DAYS(H16,G16)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="J16" s="3">
-        <f>DATEDIF(0,I16,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K16" s="3">
-        <f>DATEDIF(0,I16,"ym")</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="L16" s="3">
@@ -1178,27 +1229,27 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <f>MONTH(G17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B17" s="2">
-        <f>DAY(G17)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C17" s="2">
-        <f>YEAR(G17)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D17" s="2">
-        <f>MONTH(H17)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="E17" s="2">
-        <f>DAY(H17)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="F17" s="2">
-        <f>YEAR(H17)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G17" s="1">
@@ -1208,15 +1259,15 @@
         <v>36858</v>
       </c>
       <c r="I17" s="2">
-        <f>_xlfn.DAYS(H17,G17)</f>
+        <f t="shared" si="6"/>
         <v>252</v>
       </c>
       <c r="J17" s="3">
-        <f>DATEDIF(0,I17,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K17" s="3">
-        <f>DATEDIF(0,I17,"ym")</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="L17" s="3">
@@ -1225,27 +1276,27 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <f>MONTH(G18)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B18" s="2">
-        <f>DAY(G18)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C18" s="2">
-        <f>YEAR(G18)</f>
+        <f t="shared" si="2"/>
         <v>1999</v>
       </c>
       <c r="D18" s="2">
-        <f>MONTH(H18)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <f>DAY(H18)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <f>YEAR(H18)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G18" s="1">
@@ -1255,15 +1306,15 @@
         <v>36526</v>
       </c>
       <c r="I18" s="2">
-        <f>_xlfn.DAYS(H18,G18)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J18" s="3">
-        <f>DATEDIF(0,I18,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K18" s="3">
-        <f>DATEDIF(0,I18,"ym")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L18" s="3">
@@ -1272,27 +1323,27 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <f>MONTH(G19)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B19" s="2">
-        <f>DAY(G19)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C19" s="2">
-        <f>YEAR(G19)</f>
+        <f t="shared" si="2"/>
         <v>1999</v>
       </c>
       <c r="D19" s="2">
-        <f>MONTH(H19)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E19" s="2">
-        <f>DAY(H19)</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="F19" s="2">
-        <f>YEAR(H19)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G19" s="1">
@@ -1302,15 +1353,15 @@
         <v>36585</v>
       </c>
       <c r="I19" s="2">
-        <f>_xlfn.DAYS(H19,G19)</f>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="J19" s="3">
-        <f>DATEDIF(0,I19,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K19" s="3">
-        <f>DATEDIF(0,I19,"ym")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L19" s="3">
@@ -1319,27 +1370,27 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <f>MONTH(G20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20" s="2">
-        <f>DAY(G20)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C20" s="2">
-        <f>YEAR(G20)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D20" s="2">
-        <f>MONTH(H20)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E20" s="2">
-        <f>DAY(H20)</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="F20" s="2">
-        <f>YEAR(H20)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G20" s="1">
@@ -1349,15 +1400,15 @@
         <v>36585</v>
       </c>
       <c r="I20" s="2">
-        <f>_xlfn.DAYS(H20,G20)</f>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="J20" s="3">
-        <f>DATEDIF(0,I20,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K20" s="3">
-        <f>DATEDIF(0,I20,"ym")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L20" s="3">
@@ -1367,27 +1418,27 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <f>MONTH(G21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B21" s="2">
-        <f>DAY(G21)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C21" s="2">
-        <f>YEAR(G21)</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D21" s="2">
-        <f>MONTH(H21)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E21" s="2">
-        <f>DAY(H21)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="F21" s="2">
-        <f>YEAR(H21)</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="G21" s="1">
@@ -1397,15 +1448,15 @@
         <v>36599</v>
       </c>
       <c r="I21" s="2">
-        <f>_xlfn.DAYS(H21,G21)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="J21" s="3">
-        <f>DATEDIF(0,I21,"y")</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K21" s="3">
-        <f>DATEDIF(0,I21,"ym")</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L21" s="3">
@@ -1414,27 +1465,27 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <f>MONTH(G22)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B22" s="2">
-        <f>DAY(G22)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C22" s="2">
-        <f>YEAR(G22)</f>
+        <f t="shared" si="2"/>
         <v>1901</v>
       </c>
       <c r="D22" s="2">
-        <f>MONTH(H22)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E22" s="2">
-        <f>DAY(H22)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F22" s="2">
-        <f>YEAR(H22)</f>
+        <f t="shared" si="5"/>
         <v>1903</v>
       </c>
       <c r="G22" s="1">
@@ -1444,7 +1495,7 @@
         <v>1278</v>
       </c>
       <c r="I22" s="2">
-        <f>_xlfn.DAYS(H22,G22)</f>
+        <f t="shared" si="6"/>
         <v>731</v>
       </c>
       <c r="J22" s="3">
@@ -1459,27 +1510,27 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <f>MONTH(G23)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B23" s="2">
-        <f>DAY(G23)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C23" s="2">
-        <f>YEAR(G23)</f>
+        <f t="shared" si="2"/>
         <v>1903</v>
       </c>
       <c r="D23" s="2">
-        <f>MONTH(H23)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="E23" s="2">
-        <f>DAY(H23)</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="F23" s="2">
-        <f>YEAR(H23)</f>
+        <f t="shared" si="5"/>
         <v>1905</v>
       </c>
       <c r="G23" s="1">
@@ -1489,11 +1540,11 @@
         <v>2192</v>
       </c>
       <c r="I23" s="2">
-        <f>_xlfn.DAYS(H23,G23)</f>
+        <f t="shared" si="6"/>
         <v>822</v>
       </c>
       <c r="J23" s="3">
-        <f>DATEDIF(0,I23,"y")</f>
+        <f t="shared" ref="J23:J35" si="9">DATEDIF(0,I23,"y")</f>
         <v>2</v>
       </c>
       <c r="K23" s="3">
@@ -1505,27 +1556,27 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <f>MONTH(G24)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B24" s="2">
-        <f>DAY(G24)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C24" s="2">
-        <f>YEAR(G24)</f>
+        <f t="shared" si="2"/>
         <v>1985</v>
       </c>
       <c r="D24" s="2">
-        <f>MONTH(H24)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E24" s="2">
-        <f>DAY(H24)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F24" s="2">
-        <f>YEAR(H24)</f>
+        <f t="shared" si="5"/>
         <v>1988</v>
       </c>
       <c r="G24" s="1">
@@ -1535,15 +1586,15 @@
         <v>32340</v>
       </c>
       <c r="I24" s="2">
-        <f>_xlfn.DAYS(H24,G24)</f>
+        <f t="shared" si="6"/>
         <v>1189</v>
       </c>
       <c r="J24" s="3">
-        <f>DATEDIF(0,I24,"y")</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K24" s="3">
-        <f>DATEDIF(0,I24,"ym")</f>
+        <f t="shared" ref="K24:K32" si="10">DATEDIF(0,I24,"ym")</f>
         <v>3</v>
       </c>
       <c r="L24" s="3">
@@ -1552,27 +1603,27 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f>MONTH(G25)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B25" s="2">
-        <f>DAY(G25)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C25" s="2">
-        <f>YEAR(G25)</f>
+        <f t="shared" si="2"/>
         <v>1908</v>
       </c>
       <c r="D25" s="2">
-        <f>MONTH(H25)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E25" s="2">
-        <f>DAY(H25)</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="F25" s="2">
-        <f>YEAR(H25)</f>
+        <f t="shared" si="5"/>
         <v>1915</v>
       </c>
       <c r="G25" s="1">
@@ -1582,209 +1633,1467 @@
         <v>5510</v>
       </c>
       <c r="I25" s="2">
-        <f>_xlfn.DAYS(H25,G25)</f>
+        <f t="shared" si="6"/>
         <v>2528</v>
       </c>
       <c r="J25" s="3">
-        <f>DATEDIF(0,I25,"y")</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="K25" s="3">
-        <f>DATEDIF(0,I25,"ym")</f>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="L25" s="3">
-        <f>DATEDIF(0,I25,"md")</f>
+        <f t="shared" ref="L25:L32" si="11">DATEDIF(0,I25,"md")</f>
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="5"/>
+        <v>2000</v>
+      </c>
+      <c r="G26" s="1">
+        <v>36566</v>
+      </c>
+      <c r="H26" s="1">
+        <v>36587</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="11"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G27" s="1">
+        <v>29222</v>
+      </c>
+      <c r="H27" s="1">
+        <v>29279</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" ref="I27" si="12">_xlfn.DAYS(H27,G27)</f>
+        <v>57</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="11"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G28" s="1">
+        <v>29222</v>
+      </c>
+      <c r="H28" s="1">
+        <v>29280</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" ref="I28:I35" si="13">_xlfn.DAYS(H28,G28)</f>
+        <v>58</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="11"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G29" s="7">
+        <v>29250</v>
+      </c>
+      <c r="H29" s="7">
+        <v>29279</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="13"/>
+        <v>29</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="11"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G30" s="1">
+        <v>29251</v>
+      </c>
+      <c r="H30" s="1">
+        <v>29280</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="13"/>
+        <v>29</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="11"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G31" s="1">
+        <v>29279</v>
+      </c>
+      <c r="H31" s="1">
+        <v>29281</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G32" s="1">
+        <v>29280</v>
+      </c>
+      <c r="H32" s="1">
+        <v>29281</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G33" s="1">
+        <v>29280</v>
+      </c>
+      <c r="H33" s="1">
+        <v>29309</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="13"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G34" s="1">
+        <v>29280</v>
+      </c>
+      <c r="H34" s="1">
+        <v>29310</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="2"/>
+        <v>1980</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="5"/>
+        <v>1980</v>
+      </c>
+      <c r="G35" s="1">
+        <v>29280</v>
+      </c>
+      <c r="H35" s="1">
+        <v>29311</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="13"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1492</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2">
+        <v>15</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I36" s="2">
+        <v>193986</v>
+      </c>
+      <c r="J36" s="3">
+        <v>531</v>
+      </c>
+      <c r="K36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2">
+        <v>31</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1517</v>
+      </c>
+      <c r="D37" s="2">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I37" s="2">
+        <v>184767</v>
+      </c>
+      <c r="J37" s="3">
+        <v>505</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+      <c r="L37" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1492</v>
+      </c>
+      <c r="D38" s="2">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2">
+        <v>15</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I38" s="2">
+        <v>194103</v>
+      </c>
+      <c r="J38" s="3">
+        <v>531</v>
+      </c>
+      <c r="K38" s="3">
+        <v>5</v>
+      </c>
+      <c r="L38" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2">
+        <v>31</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1685</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2">
+        <v>15</v>
+      </c>
+      <c r="F39" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I39" s="2">
+        <v>123619</v>
+      </c>
+      <c r="J39" s="3">
+        <v>338</v>
+      </c>
+      <c r="K39" s="3">
+        <v>5</v>
+      </c>
+      <c r="L39" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>7</v>
+      </c>
+      <c r="B40" s="4">
+        <v>4</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1776</v>
+      </c>
+      <c r="D40" s="4">
+        <v>9</v>
+      </c>
+      <c r="E40" s="4">
+        <v>15</v>
+      </c>
+      <c r="F40" s="4">
+        <v>2023</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="5">
+        <v>45184</v>
+      </c>
+      <c r="I40" s="4">
+        <v>90287</v>
+      </c>
+      <c r="J40" s="4">
+        <v>247</v>
+      </c>
+      <c r="K40" s="4">
+        <v>2</v>
+      </c>
+      <c r="L40" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>12</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1805</v>
+      </c>
+      <c r="D41" s="2">
+        <v>9</v>
+      </c>
+      <c r="E41" s="2">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I41" s="2">
+        <v>79544</v>
+      </c>
+      <c r="J41" s="2">
+        <v>217</v>
+      </c>
+      <c r="K41" s="3">
+        <v>9</v>
+      </c>
+      <c r="L41" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2">
+        <v>6</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1830</v>
+      </c>
+      <c r="D42" s="2">
+        <v>9</v>
+      </c>
+      <c r="E42" s="2">
+        <v>15</v>
+      </c>
+      <c r="F42" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I42" s="2">
+        <v>70654</v>
+      </c>
+      <c r="J42" s="3">
+        <v>193</v>
+      </c>
+      <c r="K42" s="3">
+        <v>5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>537</v>
+      </c>
+      <c r="D43" s="2">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2">
+        <v>15</v>
+      </c>
+      <c r="F43" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I43" s="2">
+        <v>543005</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1486</v>
+      </c>
+      <c r="K43" s="3">
+        <v>8</v>
+      </c>
+      <c r="L43" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2">
+        <v>15</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D44" s="2">
+        <v>7</v>
+      </c>
+      <c r="E44" s="2">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2076</v>
+      </c>
+      <c r="G44" s="1">
+        <v>45184</v>
+      </c>
+      <c r="H44" s="1">
+        <v>64470</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" ref="I44:I45" si="14">_xlfn.DAYS(H44,G44)</f>
+        <v>19286</v>
+      </c>
+      <c r="J44" s="3">
+        <f>DATEDIF(0,I44,"y")</f>
+        <v>52</v>
+      </c>
+      <c r="K44" s="3">
+        <f>DATEDIF(0,I44,"ym")</f>
+        <v>9</v>
+      </c>
+      <c r="L44" s="3">
+        <f>DATEDIF(0,I44,"md")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>9</v>
+      </c>
+      <c r="B45" s="2">
+        <v>15</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2">
+        <v>6</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2030</v>
+      </c>
+      <c r="G45" s="1">
+        <v>45184</v>
+      </c>
+      <c r="H45" s="1">
+        <v>47579</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="14"/>
+        <v>2395</v>
+      </c>
+      <c r="J45" s="3">
+        <f>DATEDIF(0,I45,"y")</f>
+        <v>6</v>
+      </c>
+      <c r="K45" s="3">
+        <f>DATEDIF(0,I45,"ym")</f>
+        <v>6</v>
+      </c>
+      <c r="L45" s="3">
+        <f>DATEDIF(0,I45,"md")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>9</v>
+      </c>
+      <c r="B46" s="2">
+        <v>15</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2">
+        <v>2037</v>
+      </c>
+      <c r="G46" s="1">
+        <v>45184</v>
+      </c>
+      <c r="H46" s="1">
+        <v>50041</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" ref="I46:I47" si="15">_xlfn.DAYS(H46,G46)</f>
+        <v>4857</v>
+      </c>
+      <c r="J46" s="3">
+        <f>DATEDIF(0,I46,"y")</f>
+        <v>13</v>
+      </c>
+      <c r="K46" s="3">
+        <f>DATEDIF(0,I46,"ym")</f>
+        <v>3</v>
+      </c>
+      <c r="L46" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>9</v>
+      </c>
+      <c r="B47" s="2">
+        <v>15</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D47" s="2">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2">
+        <v>6</v>
+      </c>
+      <c r="F47" s="2">
+        <v>2093</v>
+      </c>
+      <c r="G47" s="1">
+        <v>45184</v>
+      </c>
+      <c r="H47" s="1">
+        <v>70590</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="15"/>
+        <v>25406</v>
+      </c>
+      <c r="J47" s="3">
+        <f>DATEDIF(0,I47,"y")</f>
+        <v>69</v>
+      </c>
+      <c r="K47" s="3">
+        <f>DATEDIF(0,I47,"ym")</f>
+        <v>6</v>
+      </c>
+      <c r="L47" s="3">
+        <f>DATEDIF(0,I47,"md")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2">
+        <v>6</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1893</v>
+      </c>
+      <c r="D48" s="2">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2">
+        <v>15</v>
+      </c>
+      <c r="F48" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I48" s="2">
+        <v>47643</v>
+      </c>
+      <c r="J48" s="3">
+        <v>130</v>
+      </c>
+      <c r="K48" s="3">
+        <v>5</v>
+      </c>
+      <c r="L48" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <f t="shared" ref="A49" si="16">MONTH(G49)</f>
+        <v>1</v>
+      </c>
+      <c r="B49" s="2">
+        <f t="shared" ref="B49" si="17">DAY(G49)</f>
+        <v>30</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" ref="C49" si="18">YEAR(G49)</f>
+        <v>1980</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" ref="D49" si="19">MONTH(H49)</f>
+        <v>3</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" ref="E49" si="20">DAY(H49)</f>
+        <v>5</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" ref="F49" si="21">YEAR(H49)</f>
+        <v>2000</v>
+      </c>
+      <c r="G49" s="7">
+        <v>29250</v>
+      </c>
+      <c r="H49" s="7">
+        <v>36590</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" ref="I49" si="22">_xlfn.DAYS(H49,G49)</f>
+        <v>7340</v>
+      </c>
+      <c r="J49" s="3">
+        <f>DATEDIF(0,I49,"y")</f>
+        <v>20</v>
+      </c>
+      <c r="K49" s="3">
+        <f>DATEDIF(0,I49,"ym")</f>
+        <v>1</v>
+      </c>
+      <c r="L49" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <f t="shared" ref="A50" si="23">MONTH(G50)</f>
+        <v>1</v>
+      </c>
+      <c r="B50" s="2">
+        <f t="shared" ref="B50" si="24">DAY(G50)</f>
+        <v>30</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" ref="C50" si="25">YEAR(G50)</f>
+        <v>2000</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" ref="D50" si="26">MONTH(H50)</f>
+        <v>3</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" ref="E50" si="27">DAY(H50)</f>
+        <v>5</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" ref="F50" si="28">YEAR(H50)</f>
+        <v>2000</v>
+      </c>
+      <c r="G50" s="7">
+        <v>36555</v>
+      </c>
+      <c r="H50" s="7">
+        <v>36590</v>
+      </c>
+      <c r="I50" s="2">
+        <v>35</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1</v>
+      </c>
+      <c r="L50" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <f t="shared" ref="A51" si="29">MONTH(G51)</f>
+        <v>3</v>
+      </c>
+      <c r="B51" s="2">
+        <f t="shared" ref="B51" si="30">DAY(G51)</f>
+        <v>31</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" ref="C51" si="31">YEAR(G51)</f>
+        <v>1987</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" ref="D51" si="32">MONTH(H51)</f>
+        <v>5</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" ref="E51" si="33">DAY(H51)</f>
+        <v>5</v>
+      </c>
+      <c r="F51" s="2">
+        <f t="shared" ref="F51" si="34">YEAR(H51)</f>
+        <v>1987</v>
+      </c>
+      <c r="G51" s="7">
+        <v>31867</v>
+      </c>
+      <c r="H51" s="7">
+        <v>31902</v>
+      </c>
+      <c r="I51" s="2">
+        <v>36</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <v>1</v>
+      </c>
+      <c r="L51" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <f t="shared" ref="A52" si="35">MONTH(G52)</f>
+        <v>1</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" ref="B52" si="36">DAY(G52)</f>
+        <v>31</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" ref="C52" si="37">YEAR(G52)</f>
+        <v>1987</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" ref="D52" si="38">MONTH(H52)</f>
+        <v>3</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" ref="E52" si="39">DAY(H52)</f>
+        <v>5</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" ref="F52" si="40">YEAR(H52)</f>
+        <v>1987</v>
+      </c>
+      <c r="G52" s="7">
+        <v>31808</v>
+      </c>
+      <c r="H52" s="7">
+        <v>31841</v>
+      </c>
+      <c r="I52" s="2">
+        <v>36</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <v>1</v>
+      </c>
+      <c r="L52" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>3</v>
+      </c>
+      <c r="B53" s="6">
+        <v>5</v>
+      </c>
+      <c r="C53" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D53" s="6">
+        <v>5</v>
+      </c>
+      <c r="E53" s="6">
+        <v>19</v>
+      </c>
+      <c r="F53" s="6">
+        <v>1930</v>
+      </c>
+      <c r="G53" s="7">
+        <v>36590</v>
+      </c>
+      <c r="H53" s="7">
+        <v>11097</v>
+      </c>
+      <c r="I53" s="6">
+        <v>25493</v>
+      </c>
+      <c r="J53" s="6">
+        <v>69</v>
+      </c>
+      <c r="K53" s="6">
+        <v>9</v>
+      </c>
+      <c r="L53" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>8</v>
+      </c>
+      <c r="B54" s="2">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2">
+        <v>17</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1967</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="1">
+        <v>24783</v>
+      </c>
+      <c r="I54" s="2">
+        <v>353279</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1966</v>
+      </c>
+      <c r="K54" s="2">
+        <v>5</v>
+      </c>
+      <c r="L54" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>0</v>
+      </c>
+      <c r="B55" s="2">
+        <v>22</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D55" s="2">
+        <v>9</v>
+      </c>
+      <c r="E55" s="2">
+        <v>15</v>
+      </c>
+      <c r="F55" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I55" s="2">
+        <v>14481</v>
+      </c>
+      <c r="J55" s="3">
+        <v>39</v>
+      </c>
+      <c r="K55" s="3">
+        <v>7</v>
+      </c>
+      <c r="L55" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>13</v>
+      </c>
+      <c r="B56" s="2">
+        <v>19</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1956</v>
+      </c>
+      <c r="D56" s="2">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2">
+        <v>15</v>
+      </c>
+      <c r="F56" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="1">
+        <v>45184</v>
+      </c>
+      <c r="I56" s="2">
+        <v>24376</v>
+      </c>
+      <c r="J56" s="3">
+        <v>66</v>
+      </c>
+      <c r="K56" s="3">
+        <v>8</v>
+      </c>
+      <c r="L56" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>1</v>
+      </c>
+      <c r="B57" s="2">
+        <v>17</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1963</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>22</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1984</v>
+      </c>
+      <c r="G57" s="1">
+        <v>23028</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="2">
+        <v>7875</v>
+      </c>
+      <c r="J57" s="3">
+        <v>21</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>1</v>
+      </c>
+      <c r="B58" s="2">
+        <v>17</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1947</v>
+      </c>
+      <c r="D58" s="2">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2">
+        <v>19</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1956</v>
+      </c>
+      <c r="G58" s="1">
+        <v>17184</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" s="2">
+        <v>3524</v>
+      </c>
+      <c r="J58" s="3">
+        <v>9</v>
+      </c>
+      <c r="K58" s="3">
+        <v>11</v>
+      </c>
+      <c r="L58" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>99</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B59" s="2">
         <v>99</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C59" s="2">
         <v>99</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D59" s="2">
         <v>99</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E59" s="2">
         <v>99</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F59" s="2">
         <v>99</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
+      <c r="G59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2">
         <v>99</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J59" s="3">
         <v>99</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K59" s="2">
         <v>99</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L59" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H27" s="1"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H28" s="1"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H29" s="1"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H30" s="1"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H31" s="1"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H32" s="1"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H33" s="1"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H34" s="1"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H35" s="1"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H36" s="1"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H37" s="1"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H38" s="1"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H39" s="1"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H40" s="1"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H41" s="1"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H42" s="1"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H43" s="1"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H44" s="1"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H45" s="1"/>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H46" s="1"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H47" s="1"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H48" s="1"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H49" s="1"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H50" s="1"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H51" s="1"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H52" s="1"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H53" s="1"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H54" s="1"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H55" s="1"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H56" s="1"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H57" s="1"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H58" s="1"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H59" s="1"/>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H60" s="1"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H61" s="1"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H62" s="1"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H63" s="1"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H64" s="1"/>
       <c r="J64" s="3"/>
     </row>
@@ -2048,7 +3357,140 @@
       <c r="H129" s="1"/>
       <c r="J129" s="3"/>
     </row>
+    <row r="130" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H130" s="1"/>
+      <c r="J130" s="3"/>
+    </row>
+    <row r="131" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H131" s="1"/>
+      <c r="J131" s="3"/>
+    </row>
+    <row r="132" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H132" s="1"/>
+      <c r="J132" s="3"/>
+    </row>
+    <row r="133" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H133" s="1"/>
+      <c r="J133" s="3"/>
+    </row>
+    <row r="134" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H134" s="1"/>
+      <c r="J134" s="3"/>
+    </row>
+    <row r="135" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H135" s="1"/>
+      <c r="J135" s="3"/>
+    </row>
+    <row r="136" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H136" s="1"/>
+      <c r="J136" s="3"/>
+    </row>
+    <row r="137" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H137" s="1"/>
+      <c r="J137" s="3"/>
+    </row>
+    <row r="138" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H138" s="1"/>
+      <c r="J138" s="3"/>
+    </row>
+    <row r="139" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H139" s="1"/>
+      <c r="J139" s="3"/>
+    </row>
+    <row r="140" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H140" s="1"/>
+      <c r="J140" s="3"/>
+    </row>
+    <row r="141" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H141" s="1"/>
+      <c r="J141" s="3"/>
+    </row>
+    <row r="142" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H142" s="1"/>
+      <c r="J142" s="3"/>
+    </row>
+    <row r="143" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H143" s="1"/>
+      <c r="J143" s="3"/>
+    </row>
+    <row r="144" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H144" s="1"/>
+      <c r="J144" s="3"/>
+    </row>
+    <row r="145" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H145" s="1"/>
+      <c r="J145" s="3"/>
+    </row>
+    <row r="146" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H146" s="1"/>
+      <c r="J146" s="3"/>
+    </row>
+    <row r="147" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H147" s="1"/>
+      <c r="J147" s="3"/>
+    </row>
+    <row r="148" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H148" s="1"/>
+      <c r="J148" s="3"/>
+    </row>
+    <row r="149" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H149" s="1"/>
+      <c r="J149" s="3"/>
+    </row>
+    <row r="150" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H150" s="1"/>
+      <c r="J150" s="3"/>
+    </row>
+    <row r="151" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H151" s="1"/>
+      <c r="J151" s="3"/>
+    </row>
+    <row r="152" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H152" s="1"/>
+      <c r="J152" s="3"/>
+    </row>
+    <row r="153" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H153" s="1"/>
+      <c r="J153" s="3"/>
+    </row>
+    <row r="154" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H154" s="1"/>
+      <c r="J154" s="3"/>
+    </row>
+    <row r="155" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H155" s="1"/>
+      <c r="J155" s="3"/>
+    </row>
+    <row r="156" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H156" s="1"/>
+      <c r="J156" s="3"/>
+    </row>
+    <row r="157" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H157" s="1"/>
+      <c r="J157" s="3"/>
+    </row>
+    <row r="158" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H158" s="1"/>
+      <c r="J158" s="3"/>
+    </row>
+    <row r="159" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H159" s="1"/>
+      <c r="J159" s="3"/>
+    </row>
+    <row r="160" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H160" s="1"/>
+      <c r="J160" s="3"/>
+    </row>
+    <row r="161" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H161" s="1"/>
+      <c r="J161" s="3"/>
+    </row>
+    <row r="162" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H162" s="1"/>
+      <c r="J162" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>